<commit_message>
Test cases added as suggested
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/ListingPageTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/ListingPageTestData.xlsx
@@ -4,20 +4,35 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="bannerImg" sheetId="4" r:id="rId1"/>
     <sheet name="bannerTexts" sheetId="1" r:id="rId2"/>
     <sheet name="quickFilter" sheetId="2" r:id="rId3"/>
     <sheet name="sortBy" sheetId="5" r:id="rId4"/>
+    <sheet name="article" sheetId="7" r:id="rId5"/>
+    <sheet name="filter" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>testcase</t>
   </si>
@@ -34,13 +49,13 @@
     <t>expectedText</t>
   </si>
   <si>
-    <t>Verify the banner heading</t>
+    <t>Verify the banner heading text</t>
   </si>
   <si>
     <t>Allergy Relief Medication &amp; Anti-Itch Products</t>
   </si>
   <si>
-    <t>Verify the banner sub-heading</t>
+    <t>Verify the banner sub-heading text</t>
   </si>
   <si>
     <t>Get allergy relief with the best allergy medicine from BENADRYL® and soothe your itchy skin with BENADRYL®’s selection of anti-itch topical products.</t>
@@ -77,12 +92,147 @@
   </si>
   <si>
     <t>Featured</t>
+  </si>
+  <si>
+    <t>altTxt</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>Verify dosing guide article</t>
+  </si>
+  <si>
+    <t>Benadryl dosing for children and adults</t>
+  </si>
+  <si>
+    <t>https://www.benadryl.com/benadryl-dosing-guide</t>
+  </si>
+  <si>
+    <t>Verify cold and allergies article</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Woman with cold or allergies</t>
+  </si>
+  <si>
+    <t>https://www.benadryl.com/cold/cold-or-allergies</t>
+  </si>
+  <si>
+    <t>filterText</t>
+  </si>
+  <si>
+    <t>subFilter</t>
+  </si>
+  <si>
+    <t>Verify Ages filter for 2+</t>
+  </si>
+  <si>
+    <t>Ages</t>
+  </si>
+  <si>
+    <t>2+</t>
+  </si>
+  <si>
+    <t>Verify Ages filter for 6+</t>
+  </si>
+  <si>
+    <t>6+</t>
+  </si>
+  <si>
+    <t>Verify Ages filter for 6-11</t>
+  </si>
+  <si>
+    <t>6-11</t>
+  </si>
+  <si>
+    <t>Verify Ages filter 12+</t>
+  </si>
+  <si>
+    <t>12+</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Itchy Nose and/or Throat</t>
+  </si>
+  <si>
+    <t>Symptom</t>
+  </si>
+  <si>
+    <t>Itchy Nose and/or Throat</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Itchy Skin</t>
+  </si>
+  <si>
+    <t>Itchy Skin</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Itchy, Watery Eyes</t>
+  </si>
+  <si>
+    <t>Itchy, Watery Eyes</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Nasal Congestion</t>
+  </si>
+  <si>
+    <t>Nasal Congestion</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Runny Nose</t>
+  </si>
+  <si>
+    <t>Runny Nose</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Scrapes &amp; Minor Cuts</t>
+  </si>
+  <si>
+    <t>Scrapes &amp; Minor Cuts</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Sinus Pressure</t>
+  </si>
+  <si>
+    <t>Sinus Pressure</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Sneezing</t>
+  </si>
+  <si>
+    <t>Sneezing</t>
+  </si>
+  <si>
+    <t>Verify Symptom filter for Sunburn &amp; Minor Burns</t>
+  </si>
+  <si>
+    <t>Sunburn &amp; Minor Burns</t>
+  </si>
+  <si>
+    <t>Verify Category filter for Adult Products</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Adult Products</t>
+  </si>
+  <si>
+    <t>Verify Category filter for Children's Products</t>
+  </si>
+  <si>
+    <t>Children's Products</t>
+  </si>
+  <si>
+    <t>Verify Category filter for Topical Products</t>
+  </si>
+  <si>
+    <t>Topical Products</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -690,11 +840,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,7 +1172,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1056,8 +1208,8 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -1081,7 +1233,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1091,8 +1243,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+    <row r="3" ht="30" spans="1:3">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1114,12 +1266,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C4"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="29.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="34.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="10.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="21.5714285714286" customWidth="1"/>
   </cols>
@@ -1180,7 +1332,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -1227,4 +1379,333 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="29.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="9.57142857142857" customWidth="1"/>
+    <col min="3" max="3" width="47.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://www.benadryl.com/benadryl-dosing-guide"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://www.benadryl.com/cold/cold-or-allergies"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="49.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="35.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="24.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>